<commit_message>
Initial Commit of PCB files
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\x399 Burn In\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\x399 Burn In\x399_Burn_In\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491C7B7A-86A0-4993-8674-AD0C832D7F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB67F06-798D-4FAC-9A35-3826D7FAD356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
   <si>
     <t>Vref</t>
   </si>
@@ -264,9 +264,6 @@
     <t>Imisc</t>
   </si>
   <si>
-    <t>Src?</t>
-  </si>
-  <si>
     <t>Istart</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>Redo sheet?</t>
+  </si>
+  <si>
+    <t>Istartup</t>
   </si>
 </sst>
 </file>
@@ -417,10 +417,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,7 +726,7 @@
   <dimension ref="B1:R86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,36 +741,36 @@
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="I4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="P4" s="12" t="s">
+      <c r="J4" s="13"/>
+      <c r="P4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D5" s="5" t="s">
@@ -1857,10 +1857,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B11F8B8-99A9-466C-98A9-415FD47DA591}">
-  <dimension ref="A3:I25"/>
+  <dimension ref="C3:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1869,14 +1869,14 @@
     <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C3" s="12" t="s">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>10</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>70</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1968,10 +1968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>75</v>
-      </c>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1992,7 +1989,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>74</v>
       </c>
@@ -2014,7 +2011,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
@@ -2035,9 +2032,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
       <c r="G12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H12">
         <f>H6/H5</f>
@@ -2047,7 +2044,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="G13" s="2" t="s">
         <v>71</v>
       </c>
@@ -2059,7 +2056,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
       <c r="G14" s="2" t="s">
         <v>72</v>
       </c>
@@ -2071,7 +2068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
       <c r="G15" s="2" t="s">
         <v>73</v>
       </c>
@@ -2083,9 +2080,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H16">
         <f>H10+H13+H15</f>
@@ -2097,7 +2094,7 @@
     </row>
     <row r="17" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H17">
         <f>H12-H16</f>
@@ -2109,9 +2106,9 @@
     </row>
     <row r="18" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H18" s="13">
+        <v>78</v>
+      </c>
+      <c r="H18" s="12">
         <f>H17/H12</f>
         <v>0.12159999999999993</v>
       </c>
@@ -2121,7 +2118,7 @@
     </row>
     <row r="19" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H19">
         <f>H15+H14+H10</f>
@@ -2136,7 +2133,7 @@
     </row>
     <row r="21" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G21" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H21">
         <f>H16*H5</f>
@@ -2148,7 +2145,7 @@
     </row>
     <row r="22" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G22" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H22">
         <f>H19*H5</f>
@@ -2162,10 +2159,22 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24">
+        <f>H21/H5</f>
+        <v>0.87840000000000007</v>
+      </c>
     </row>
     <row r="25" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25">
+        <f>H22/H6</f>
+        <v>0.19840000000000002</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>